<commit_message>
Add ChIP-Exo data; update iModulon categories
</commit_message>
<xml_diff>
--- a/data/regulation/gao_dataset_s4.xlsx
+++ b/data/regulation/gao_dataset_s4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cam/Projects/precise2/data/regulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B298B02D-619A-304B-B9D3-841A1AD83BD1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B625C84-34E5-2C41-9F15-8758CCC04492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{036DBEDF-A659-BE48-9F25-A0A950D476E2}"/>
   </bookViews>
@@ -4211,7 +4211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80ED76D9-DB5D-CE4D-A705-850876D8660C}">
   <dimension ref="A1:J1203"/>
   <sheetViews>
-    <sheetView topLeftCell="A710" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B743" sqref="B743:E743"/>
     </sheetView>
   </sheetViews>
@@ -21239,8 +21239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1771D553-BE2E-9646-82B6-BDBE79E5E02A}">
   <dimension ref="A1:E589"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E590" sqref="E590"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22576,7 +22576,7 @@
         <v>3208803</v>
       </c>
       <c r="B79">
-        <v>320843</v>
+        <v>3208843</v>
       </c>
       <c r="C79">
         <v>12.3</v>

</xml_diff>